<commit_message>
front + journal léonard
</commit_message>
<xml_diff>
--- a/documentation/Journal/3_1_Léonard_Journal.xlsx
+++ b/documentation/Journal/3_1_Léonard_Journal.xlsx
@@ -5,10 +5,10 @@
   <workbookPr checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eduetatfr-my.sharepoint.com/personal/gabriel_beer_studentfr_ch/Documents/EMF/Informatique EMF/Troisième année/306/306project-G4/documentation/Journal/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leo/Downloads/306project-G4/documentation/Journal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{4C909ACB-C3FE-0D42-B97D-B7AD9923E282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{27CA9FE2-D3D5-2945-AD20-796D160E7007}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA711A2C-3A96-7A41-941E-E40EA67F6D8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="22">
   <si>
     <t>Insérer les lignes au-dessus de celle-ci !</t>
   </si>
@@ -104,6 +104,24 @@
   </si>
   <si>
     <t>Mettre a jour le journal</t>
+  </si>
+  <si>
+    <t>Bien travaillé aujourd'hui, journée productive</t>
+  </si>
+  <si>
+    <t>finis la maquette</t>
+  </si>
+  <si>
+    <t>développer l'app en code</t>
+  </si>
+  <si>
+    <t>corriger le use case</t>
+  </si>
+  <si>
+    <t>créer des user story</t>
+  </si>
+  <si>
+    <t xml:space="preserve">corriger le planning </t>
   </si>
 </sst>
 </file>
@@ -443,6 +461,10 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -451,6 +473,10 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
@@ -467,6 +493,18 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
@@ -479,64 +517,44 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1172,9 +1190,9 @@
   <dimension ref="A1:D84"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="186" zoomScaleNormal="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <pane ySplit="1" activePane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft"/>
       <selection activeCell="A5" sqref="A5:XFD5"/>
-      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
+      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1195,89 +1213,89 @@
       <c r="D1" s="27"/>
     </row>
     <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="35"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="29"/>
       <c r="D2" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="29"/>
+      <c r="C4" s="32"/>
       <c r="D4" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="30"/>
-      <c r="B5" s="30"/>
-      <c r="C5" s="31"/>
+      <c r="A5" s="31"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="33"/>
       <c r="D5" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="26">
+      <c r="A6" s="34">
         <v>46000</v>
       </c>
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="33"/>
+      <c r="C6" s="36"/>
       <c r="D6" s="7">
         <v>0.5</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A7" s="14"/>
-      <c r="B7" s="17" t="s">
+      <c r="A7" s="15"/>
+      <c r="B7" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="18"/>
+      <c r="C7" s="20"/>
       <c r="D7" s="8">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A8" s="14"/>
-      <c r="B8" s="17" t="s">
+      <c r="A8" s="15"/>
+      <c r="B8" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="18"/>
+      <c r="C8" s="20"/>
       <c r="D8" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A9" s="14"/>
-      <c r="B9" s="17" t="s">
+      <c r="A9" s="15"/>
+      <c r="B9" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="18"/>
+      <c r="C9" s="20"/>
       <c r="D9" s="8">
         <v>0.33</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A10" s="14"/>
-      <c r="B10" s="17" t="s">
+      <c r="A10" s="15"/>
+      <c r="B10" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="18"/>
+      <c r="C10" s="20"/>
       <c r="D10" s="8">
         <v>0.2</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A11" s="14"/>
+      <c r="A11" s="15"/>
       <c r="B11" s="2" t="s">
         <v>6</v>
       </c>
@@ -1290,43 +1308,65 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="14"/>
-      <c r="B12" s="19"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="21"/>
+      <c r="A12" s="15"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="26"/>
     </row>
     <row r="13" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="13"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="7"/>
+      <c r="A13" s="14">
+        <v>46006</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="18"/>
+      <c r="D13" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A14" s="14"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="8"/>
+      <c r="A14" s="15"/>
+      <c r="B14" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="20"/>
+      <c r="D14" s="8">
+        <v>4</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A15" s="14"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="8"/>
+      <c r="A15" s="15"/>
+      <c r="B15" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="20"/>
+      <c r="D15" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A16" s="14"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="8"/>
+      <c r="A16" s="15"/>
+      <c r="B16" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="20"/>
+      <c r="D16" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A17" s="14"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="8"/>
+      <c r="A17" s="15"/>
+      <c r="B17" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="20"/>
+      <c r="D17" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A18" s="14"/>
+      <c r="A18" s="15"/>
       <c r="B18" s="2" t="s">
         <v>6</v>
       </c>
@@ -1335,47 +1375,49 @@
       </c>
       <c r="D18" s="9">
         <f>SUM(D13:D17)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="14"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="21"/>
+      <c r="A19" s="15"/>
+      <c r="B19" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="25"/>
+      <c r="D19" s="26"/>
     </row>
     <row r="20" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="13"/>
-      <c r="B20" s="15"/>
-      <c r="C20" s="16"/>
+      <c r="A20" s="14"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="18"/>
       <c r="D20" s="7"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A21" s="14"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="18"/>
+      <c r="A21" s="15"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="20"/>
       <c r="D21" s="8"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A22" s="14"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="18"/>
+      <c r="A22" s="15"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="20"/>
       <c r="D22" s="8"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A23" s="14"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="18"/>
+      <c r="A23" s="15"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="20"/>
       <c r="D23" s="8"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A24" s="14"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="18"/>
+      <c r="A24" s="15"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="20"/>
       <c r="D24" s="8"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A25" s="14"/>
+      <c r="A25" s="15"/>
       <c r="B25" s="2" t="s">
         <v>6</v>
       </c>
@@ -1388,43 +1430,43 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="14"/>
-      <c r="B26" s="19"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="21"/>
+      <c r="A26" s="15"/>
+      <c r="B26" s="24"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="26"/>
     </row>
     <row r="27" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="13"/>
-      <c r="B27" s="15"/>
-      <c r="C27" s="16"/>
+      <c r="A27" s="14"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="18"/>
       <c r="D27" s="7"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A28" s="14"/>
-      <c r="B28" s="17"/>
-      <c r="C28" s="18"/>
+      <c r="A28" s="15"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="20"/>
       <c r="D28" s="8"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A29" s="14"/>
-      <c r="B29" s="17"/>
-      <c r="C29" s="18"/>
+      <c r="A29" s="15"/>
+      <c r="B29" s="19"/>
+      <c r="C29" s="20"/>
       <c r="D29" s="8"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A30" s="14"/>
-      <c r="B30" s="17"/>
-      <c r="C30" s="18"/>
+      <c r="A30" s="15"/>
+      <c r="B30" s="19"/>
+      <c r="C30" s="20"/>
       <c r="D30" s="8"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A31" s="14"/>
-      <c r="B31" s="17"/>
-      <c r="C31" s="18"/>
+      <c r="A31" s="15"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="20"/>
       <c r="D31" s="8"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A32" s="14"/>
+      <c r="A32" s="15"/>
       <c r="B32" s="2" t="s">
         <v>6</v>
       </c>
@@ -1437,43 +1479,43 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="25"/>
-      <c r="B33" s="22"/>
-      <c r="C33" s="23"/>
-      <c r="D33" s="24"/>
+      <c r="A33" s="16"/>
+      <c r="B33" s="21"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="23"/>
     </row>
     <row r="34" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="13"/>
-      <c r="B34" s="15"/>
-      <c r="C34" s="16"/>
+      <c r="A34" s="14"/>
+      <c r="B34" s="17"/>
+      <c r="C34" s="18"/>
       <c r="D34" s="7"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A35" s="14"/>
-      <c r="B35" s="17"/>
-      <c r="C35" s="18"/>
+      <c r="A35" s="15"/>
+      <c r="B35" s="19"/>
+      <c r="C35" s="20"/>
       <c r="D35" s="8"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A36" s="14"/>
-      <c r="B36" s="17"/>
-      <c r="C36" s="18"/>
+      <c r="A36" s="15"/>
+      <c r="B36" s="19"/>
+      <c r="C36" s="20"/>
       <c r="D36" s="8"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A37" s="14"/>
-      <c r="B37" s="17"/>
-      <c r="C37" s="18"/>
+      <c r="A37" s="15"/>
+      <c r="B37" s="19"/>
+      <c r="C37" s="20"/>
       <c r="D37" s="8"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A38" s="14"/>
-      <c r="B38" s="17"/>
-      <c r="C38" s="18"/>
+      <c r="A38" s="15"/>
+      <c r="B38" s="19"/>
+      <c r="C38" s="20"/>
       <c r="D38" s="8"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A39" s="14"/>
+      <c r="A39" s="15"/>
       <c r="B39" s="2" t="s">
         <v>6</v>
       </c>
@@ -1486,43 +1528,43 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="25"/>
-      <c r="B40" s="22"/>
-      <c r="C40" s="23"/>
-      <c r="D40" s="24"/>
+      <c r="A40" s="16"/>
+      <c r="B40" s="21"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="23"/>
     </row>
     <row r="41" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="13"/>
-      <c r="B41" s="15"/>
-      <c r="C41" s="16"/>
+      <c r="A41" s="14"/>
+      <c r="B41" s="17"/>
+      <c r="C41" s="18"/>
       <c r="D41" s="7"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A42" s="14"/>
-      <c r="B42" s="17"/>
-      <c r="C42" s="18"/>
+      <c r="A42" s="15"/>
+      <c r="B42" s="19"/>
+      <c r="C42" s="20"/>
       <c r="D42" s="8"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A43" s="14"/>
-      <c r="B43" s="17"/>
-      <c r="C43" s="18"/>
+      <c r="A43" s="15"/>
+      <c r="B43" s="19"/>
+      <c r="C43" s="20"/>
       <c r="D43" s="8"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A44" s="14"/>
-      <c r="B44" s="17"/>
-      <c r="C44" s="18"/>
+      <c r="A44" s="15"/>
+      <c r="B44" s="19"/>
+      <c r="C44" s="20"/>
       <c r="D44" s="8"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A45" s="14"/>
-      <c r="B45" s="17"/>
-      <c r="C45" s="18"/>
+      <c r="A45" s="15"/>
+      <c r="B45" s="19"/>
+      <c r="C45" s="20"/>
       <c r="D45" s="8"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A46" s="14"/>
+      <c r="A46" s="15"/>
       <c r="B46" s="2" t="s">
         <v>6</v>
       </c>
@@ -1535,43 +1577,43 @@
       </c>
     </row>
     <row r="47" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A47" s="25"/>
-      <c r="B47" s="22"/>
-      <c r="C47" s="23"/>
-      <c r="D47" s="24"/>
+      <c r="A47" s="16"/>
+      <c r="B47" s="21"/>
+      <c r="C47" s="22"/>
+      <c r="D47" s="23"/>
     </row>
     <row r="48" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="13"/>
-      <c r="B48" s="15"/>
-      <c r="C48" s="16"/>
+      <c r="A48" s="14"/>
+      <c r="B48" s="17"/>
+      <c r="C48" s="18"/>
       <c r="D48" s="7"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A49" s="14"/>
-      <c r="B49" s="17"/>
-      <c r="C49" s="18"/>
+      <c r="A49" s="15"/>
+      <c r="B49" s="19"/>
+      <c r="C49" s="20"/>
       <c r="D49" s="8"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A50" s="14"/>
-      <c r="B50" s="17"/>
-      <c r="C50" s="18"/>
+      <c r="A50" s="15"/>
+      <c r="B50" s="19"/>
+      <c r="C50" s="20"/>
       <c r="D50" s="8"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A51" s="14"/>
-      <c r="B51" s="17"/>
-      <c r="C51" s="18"/>
+      <c r="A51" s="15"/>
+      <c r="B51" s="19"/>
+      <c r="C51" s="20"/>
       <c r="D51" s="8"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A52" s="14"/>
-      <c r="B52" s="17"/>
-      <c r="C52" s="18"/>
+      <c r="A52" s="15"/>
+      <c r="B52" s="19"/>
+      <c r="C52" s="20"/>
       <c r="D52" s="8"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A53" s="14"/>
+      <c r="A53" s="15"/>
       <c r="B53" s="2" t="s">
         <v>6</v>
       </c>
@@ -1584,43 +1626,43 @@
       </c>
     </row>
     <row r="54" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A54" s="25"/>
-      <c r="B54" s="22"/>
-      <c r="C54" s="23"/>
-      <c r="D54" s="24"/>
+      <c r="A54" s="16"/>
+      <c r="B54" s="21"/>
+      <c r="C54" s="22"/>
+      <c r="D54" s="23"/>
     </row>
     <row r="55" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A55" s="13"/>
-      <c r="B55" s="15"/>
-      <c r="C55" s="16"/>
+      <c r="A55" s="14"/>
+      <c r="B55" s="17"/>
+      <c r="C55" s="18"/>
       <c r="D55" s="7"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A56" s="14"/>
-      <c r="B56" s="17"/>
-      <c r="C56" s="18"/>
+      <c r="A56" s="15"/>
+      <c r="B56" s="19"/>
+      <c r="C56" s="20"/>
       <c r="D56" s="8"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A57" s="14"/>
-      <c r="B57" s="17"/>
-      <c r="C57" s="18"/>
+      <c r="A57" s="15"/>
+      <c r="B57" s="19"/>
+      <c r="C57" s="20"/>
       <c r="D57" s="8"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A58" s="14"/>
-      <c r="B58" s="17"/>
-      <c r="C58" s="18"/>
+      <c r="A58" s="15"/>
+      <c r="B58" s="19"/>
+      <c r="C58" s="20"/>
       <c r="D58" s="8"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A59" s="14"/>
-      <c r="B59" s="17"/>
-      <c r="C59" s="18"/>
+      <c r="A59" s="15"/>
+      <c r="B59" s="19"/>
+      <c r="C59" s="20"/>
       <c r="D59" s="8"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A60" s="14"/>
+      <c r="A60" s="15"/>
       <c r="B60" s="2" t="s">
         <v>6</v>
       </c>
@@ -1633,43 +1675,43 @@
       </c>
     </row>
     <row r="61" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A61" s="25"/>
-      <c r="B61" s="22"/>
-      <c r="C61" s="23"/>
-      <c r="D61" s="24"/>
+      <c r="A61" s="16"/>
+      <c r="B61" s="21"/>
+      <c r="C61" s="22"/>
+      <c r="D61" s="23"/>
     </row>
     <row r="62" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A62" s="13"/>
-      <c r="B62" s="15"/>
-      <c r="C62" s="16"/>
+      <c r="A62" s="14"/>
+      <c r="B62" s="17"/>
+      <c r="C62" s="18"/>
       <c r="D62" s="7"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A63" s="14"/>
-      <c r="B63" s="17"/>
-      <c r="C63" s="18"/>
+      <c r="A63" s="15"/>
+      <c r="B63" s="19"/>
+      <c r="C63" s="20"/>
       <c r="D63" s="8"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A64" s="14"/>
-      <c r="B64" s="17"/>
-      <c r="C64" s="18"/>
+      <c r="A64" s="15"/>
+      <c r="B64" s="19"/>
+      <c r="C64" s="20"/>
       <c r="D64" s="8"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A65" s="14"/>
-      <c r="B65" s="17"/>
-      <c r="C65" s="18"/>
+      <c r="A65" s="15"/>
+      <c r="B65" s="19"/>
+      <c r="C65" s="20"/>
       <c r="D65" s="8"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A66" s="14"/>
-      <c r="B66" s="17"/>
-      <c r="C66" s="18"/>
+      <c r="A66" s="15"/>
+      <c r="B66" s="19"/>
+      <c r="C66" s="20"/>
       <c r="D66" s="8"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A67" s="14"/>
+      <c r="A67" s="15"/>
       <c r="B67" s="2" t="s">
         <v>6</v>
       </c>
@@ -1682,43 +1724,43 @@
       </c>
     </row>
     <row r="68" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A68" s="14"/>
-      <c r="B68" s="19"/>
-      <c r="C68" s="20"/>
-      <c r="D68" s="21"/>
+      <c r="A68" s="15"/>
+      <c r="B68" s="24"/>
+      <c r="C68" s="25"/>
+      <c r="D68" s="26"/>
     </row>
     <row r="69" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A69" s="13"/>
-      <c r="B69" s="15"/>
-      <c r="C69" s="16"/>
+      <c r="A69" s="14"/>
+      <c r="B69" s="17"/>
+      <c r="C69" s="18"/>
       <c r="D69" s="7"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A70" s="14"/>
-      <c r="B70" s="17"/>
-      <c r="C70" s="18"/>
+      <c r="A70" s="15"/>
+      <c r="B70" s="19"/>
+      <c r="C70" s="20"/>
       <c r="D70" s="8"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A71" s="14"/>
-      <c r="B71" s="17"/>
-      <c r="C71" s="18"/>
+      <c r="A71" s="15"/>
+      <c r="B71" s="19"/>
+      <c r="C71" s="20"/>
       <c r="D71" s="8"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A72" s="14"/>
-      <c r="B72" s="17"/>
-      <c r="C72" s="18"/>
+      <c r="A72" s="15"/>
+      <c r="B72" s="19"/>
+      <c r="C72" s="20"/>
       <c r="D72" s="8"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A73" s="14"/>
-      <c r="B73" s="17"/>
-      <c r="C73" s="18"/>
+      <c r="A73" s="15"/>
+      <c r="B73" s="19"/>
+      <c r="C73" s="20"/>
       <c r="D73" s="8"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A74" s="14"/>
+      <c r="A74" s="15"/>
       <c r="B74" s="2" t="s">
         <v>6</v>
       </c>
@@ -1731,43 +1773,43 @@
       </c>
     </row>
     <row r="75" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A75" s="25"/>
-      <c r="B75" s="22"/>
-      <c r="C75" s="23"/>
-      <c r="D75" s="24"/>
+      <c r="A75" s="16"/>
+      <c r="B75" s="21"/>
+      <c r="C75" s="22"/>
+      <c r="D75" s="23"/>
     </row>
     <row r="76" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A76" s="13"/>
-      <c r="B76" s="15"/>
-      <c r="C76" s="16"/>
+      <c r="A76" s="14"/>
+      <c r="B76" s="17"/>
+      <c r="C76" s="18"/>
       <c r="D76" s="7"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A77" s="14"/>
-      <c r="B77" s="17"/>
-      <c r="C77" s="18"/>
+      <c r="A77" s="15"/>
+      <c r="B77" s="19"/>
+      <c r="C77" s="20"/>
       <c r="D77" s="8"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A78" s="14"/>
-      <c r="B78" s="17"/>
-      <c r="C78" s="18"/>
+      <c r="A78" s="15"/>
+      <c r="B78" s="19"/>
+      <c r="C78" s="20"/>
       <c r="D78" s="8"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A79" s="14"/>
-      <c r="B79" s="17"/>
-      <c r="C79" s="18"/>
+      <c r="A79" s="15"/>
+      <c r="B79" s="19"/>
+      <c r="C79" s="20"/>
       <c r="D79" s="8"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A80" s="14"/>
-      <c r="B80" s="17"/>
-      <c r="C80" s="18"/>
+      <c r="A80" s="15"/>
+      <c r="B80" s="19"/>
+      <c r="C80" s="20"/>
       <c r="D80" s="8"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A81" s="14"/>
+      <c r="A81" s="15"/>
       <c r="B81" s="2" t="s">
         <v>6</v>
       </c>
@@ -1780,10 +1822,10 @@
       </c>
     </row>
     <row r="82" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A82" s="25"/>
-      <c r="B82" s="22"/>
-      <c r="C82" s="23"/>
-      <c r="D82" s="24"/>
+      <c r="A82" s="16"/>
+      <c r="B82" s="21"/>
+      <c r="C82" s="22"/>
+      <c r="D82" s="23"/>
     </row>
     <row r="83" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A83" s="11"/>
@@ -1793,90 +1835,19 @@
       </c>
       <c r="D83" s="12">
         <f>D11+D18+D25+D32+D39+D46+D53+D60+D67+D74+D81</f>
-        <v>4.03</v>
+        <v>12.030000000000001</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A84" s="36" t="s">
+      <c r="A84" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B84" s="36"/>
-      <c r="C84" s="36"/>
-      <c r="D84" s="36"/>
+      <c r="B84" s="13"/>
+      <c r="C84" s="13"/>
+      <c r="D84" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="82">
-    <mergeCell ref="A84:D84"/>
-    <mergeCell ref="A76:A82"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="B78:C78"/>
-    <mergeCell ref="B79:C79"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B82:D82"/>
-    <mergeCell ref="A69:A75"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B75:D75"/>
-    <mergeCell ref="A62:A68"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B68:D68"/>
-    <mergeCell ref="A55:A61"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B61:D61"/>
-    <mergeCell ref="A48:A54"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="A41:A47"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B47:D47"/>
-    <mergeCell ref="A34:A40"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="A27:A33"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="A20:A26"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="A13:A19"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B19:D19"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A4:A5"/>
@@ -1888,6 +1859,77 @@
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B12:D12"/>
+    <mergeCell ref="A13:A19"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="A20:A26"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="A27:A33"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="A34:A40"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="A41:A47"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="A48:A54"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="A55:A61"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B61:D61"/>
+    <mergeCell ref="A62:A68"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B68:D68"/>
+    <mergeCell ref="A69:A75"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B75:D75"/>
+    <mergeCell ref="A84:D84"/>
+    <mergeCell ref="A76:A82"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="B78:C78"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B82:D82"/>
   </mergeCells>
   <conditionalFormatting sqref="D6:D11">
     <cfRule type="containsText" dxfId="23" priority="23" operator="containsText" text="Terminé">
@@ -2002,26 +2044,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8afaa137-8a18-4908-97f4-35fc924e5a91">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006BD0882D7B13D249A8B88997E24B9140" ma:contentTypeVersion="14" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="3865b25f2bf2a035dbe7787239b3f11c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8afaa137-8a18-4908-97f4-35fc924e5a91" xmlns:ns3="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="718f9f7ddd2530d56a17ab9424d0abda" ns2:_="" ns3:_="">
     <xsd:import namespace="8afaa137-8a18-4908-97f4-35fc924e5a91"/>
@@ -2234,32 +2256,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1CED954-0C0B-4246-88BC-C0C5C061E08E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="8afaa137-8a18-4908-97f4-35fc924e5a91"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8C0AFF7-6D45-4588-A3CE-0506D82134A8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8afaa137-8a18-4908-97f4-35fc924e5a91">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84AEF82B-2BAE-481D-A319-B09ADD6915E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2276,4 +2293,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8C0AFF7-6D45-4588-A3CE-0506D82134A8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1CED954-0C0B-4246-88BC-C0C5C061E08E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="8afaa137-8a18-4908-97f4-35fc924e5a91"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>